<commit_message>
feat: fix issue, add vetdoc, qc to create payroll
</commit_message>
<xml_diff>
--- a/public/template/transaction/Template_Export_Transaction_Pet_Shop.xlsx
+++ b/public/template/transaction/Template_Export_Transaction_Pet_Shop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\transaction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36793C7F-B98C-4075-B88B-BBFE3D5B2DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7136A1D6-A311-4545-942F-A57990FAE9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Transaksi" sheetId="1" r:id="rId1"/>
@@ -30,18 +30,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>Dibuat Oleh</t>
-  </si>
-  <si>
-    <t>Dibuat Pada</t>
-  </si>
-  <si>
     <t>Transaction No</t>
   </si>
   <si>
-    <t>Cabang</t>
-  </si>
-  <si>
     <t>Customer Name</t>
   </si>
   <si>
@@ -55,6 +46,15 @@
   </si>
   <si>
     <t>Total Use Promo</t>
+  </si>
+  <si>
+    <t>Created At</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Branch</t>
   </si>
 </sst>
 </file>
@@ -436,56 +436,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0BD312-7EF2-F445-B81C-635468D350A0}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="17.8984375" customWidth="1"/>
-    <col min="5" max="5" width="17.69921875" customWidth="1"/>
-    <col min="6" max="6" width="16.296875" customWidth="1"/>
-    <col min="7" max="7" width="18.69921875" customWidth="1"/>
-    <col min="8" max="8" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="5" max="5" width="17.75" customWidth="1"/>
+    <col min="6" max="6" width="16.25" customWidth="1"/>
+    <col min="7" max="7" width="18.75" customWidth="1"/>
+    <col min="8" max="8" width="20.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="23.796875" customWidth="1"/>
-    <col min="11" max="11" width="15.19921875" customWidth="1"/>
-    <col min="12" max="12" width="17.19921875" customWidth="1"/>
+    <col min="10" max="10" width="23.75" customWidth="1"/>
+    <col min="11" max="11" width="15.25" customWidth="1"/>
+    <col min="12" max="12" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>

</xml_diff>